<commit_message>
RegisterPage Tests, OleDb, Enviroment.config
1.Enviroment.config
// folder needed
C:\BartlettAreTheQAs\ExcelFilesData\RegisterPageData.xlsx\
2. AccessExcelData - Exel Ole DB implemented
3. BlogRegisterPageTests - 7 Tests Added
4. Changes in RegisterPage.cs,
RegisterPageAsserter.cs,RegisterPageMap.cs
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Key</t>
   </si>
@@ -30,6 +30,57 @@
   </si>
   <si>
     <t>FullName</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>InvalidEmail</t>
+  </si>
+  <si>
+    <t>Cherry</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Register without mail</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Register already used email</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>a@a.a</t>
+  </si>
+  <si>
+    <t>Register without FullName</t>
+  </si>
+  <si>
+    <t>ejkobejko@mail.bg</t>
+  </si>
+  <si>
+    <t>B676KKK</t>
+  </si>
+  <si>
+    <t>Register without Password</t>
+  </si>
+  <si>
+    <t>Register without Confirm password</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Passwords do not match</t>
+  </si>
+  <si>
+    <t>b676KK</t>
   </si>
 </sst>
 </file>
@@ -105,13 +156,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -419,22 +471,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -456,87 +508,255 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="1:23" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -544,8 +764,20 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
+    <row r="10" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -553,8 +785,20 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -562,8 +806,20 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -571,8 +827,20 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -580,8 +848,20 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -589,8 +869,20 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -598,8 +890,20 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -607,8 +911,20 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+    </row>
+    <row r="17" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -616,8 +932,20 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -625,8 +953,20 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -634,8 +974,20 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -643,8 +995,20 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -652,8 +1016,20 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row r="22" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -661,8 +1037,20 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row r="23" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -670,8 +1058,20 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -679,8 +1079,20 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -688,8 +1100,20 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -697,8 +1121,20 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -706,8 +1142,20 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -715,8 +1163,20 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -724,8 +1184,20 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -733,8 +1205,20 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -742,8 +1226,20 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -751,8 +1247,20 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -760,8 +1268,20 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -769,8 +1289,20 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -778,8 +1310,20 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -787,8 +1331,20 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -796,8 +1352,20 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -805,8 +1373,20 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -814,8 +1394,20 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -823,8 +1415,20 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -832,8 +1436,20 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -841,8 +1457,20 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -850,8 +1478,20 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -859,8 +1499,20 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -868,8 +1520,20 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -877,8 +1541,20 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -886,8 +1562,20 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -895,8 +1583,20 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -904,8 +1604,20 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -913,8 +1625,20 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -922,8 +1646,20 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -931,8 +1667,20 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -940,8 +1688,20 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -949,8 +1709,20 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -958,8 +1730,20 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -967,8 +1751,20 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -976,8 +1772,20 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -985,8 +1793,20 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -994,8 +1814,20 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -1003,8 +1835,20 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -1012,8 +1856,20 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -1021,8 +1877,20 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -1030,8 +1898,20 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -1039,8 +1919,20 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -1048,8 +1940,20 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -1057,8 +1961,20 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -1066,8 +1982,20 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -1075,8 +2003,20 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -1084,8 +2024,20 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -1093,8 +2045,20 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -1102,8 +2066,20 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -1111,8 +2087,20 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -1120,8 +2108,20 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -1129,8 +2129,20 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -1138,8 +2150,20 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -1147,8 +2171,20 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -1157,7 +2193,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -1166,7 +2202,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -1176,8 +2212,15 @@
       <c r="K79" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1187,7 +2230,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add LoginPage and ManagePage - first try
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Key</t>
   </si>
@@ -81,13 +81,19 @@
   </si>
   <si>
     <t>b676KK</t>
+  </si>
+  <si>
+    <t>LogInValidEmail</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,7 +265,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -294,7 +299,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -470,14 +474,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
@@ -486,7 +490,7 @@
     <col min="5" max="5" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,7 +525,7 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:23" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -556,7 +560,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -589,7 +593,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -624,7 +628,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -657,7 +661,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -689,7 +693,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -721,7 +725,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -756,8 +760,16 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:23">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -777,7 +789,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23">
       <c r="A10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -798,7 +810,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23">
       <c r="A11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -819,7 +831,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23">
       <c r="A12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -840,7 +852,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23">
       <c r="A13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -861,7 +873,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23">
       <c r="A14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -882,7 +894,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23">
       <c r="A15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -903,7 +915,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23">
       <c r="A16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -924,7 +936,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23">
       <c r="A17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -945,7 +957,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23">
       <c r="A18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -966,7 +978,7 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
     </row>
-    <row r="19" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23">
       <c r="A19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -987,7 +999,7 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
     </row>
-    <row r="20" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23">
       <c r="A20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1008,7 +1020,7 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
     </row>
-    <row r="21" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23">
       <c r="A21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1029,7 +1041,7 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23">
       <c r="A22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1050,7 +1062,7 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
     </row>
-    <row r="23" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23">
       <c r="A23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1071,7 +1083,7 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
     </row>
-    <row r="24" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23">
       <c r="A24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1092,7 +1104,7 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1113,7 +1125,7 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="A26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1134,7 +1146,7 @@
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1155,7 +1167,7 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1176,7 +1188,7 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1197,7 +1209,7 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1218,7 +1230,7 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1239,7 +1251,7 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="A32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1260,7 +1272,7 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1281,7 +1293,7 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23">
       <c r="A34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1302,7 +1314,7 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="A35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1323,7 +1335,7 @@
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23">
       <c r="A36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1344,7 +1356,7 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23">
       <c r="A37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1365,7 +1377,7 @@
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23">
       <c r="A38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1386,7 +1398,7 @@
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23">
       <c r="A39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1407,7 +1419,7 @@
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23">
       <c r="A40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1428,7 +1440,7 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23">
       <c r="A41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1449,7 +1461,7 @@
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23">
       <c r="A42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1470,7 +1482,7 @@
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23">
       <c r="A43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1491,7 +1503,7 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23">
       <c r="A44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -1512,7 +1524,7 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23">
       <c r="A45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1533,7 +1545,7 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23">
       <c r="A46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1554,7 +1566,7 @@
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23">
       <c r="A47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -1575,7 +1587,7 @@
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23">
       <c r="A48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -1596,7 +1608,7 @@
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23">
       <c r="A49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -1617,7 +1629,7 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23">
       <c r="A50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -1638,7 +1650,7 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23">
       <c r="A51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -1659,7 +1671,7 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23">
       <c r="A52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -1680,7 +1692,7 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23">
       <c r="A53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -1701,7 +1713,7 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23">
       <c r="A54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -1722,7 +1734,7 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23">
       <c r="A55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -1743,7 +1755,7 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23">
       <c r="A56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -1764,7 +1776,7 @@
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23">
       <c r="A57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -1785,7 +1797,7 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23">
       <c r="A58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -1806,7 +1818,7 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23">
       <c r="A59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -1827,7 +1839,7 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23">
       <c r="A60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -1848,7 +1860,7 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23">
       <c r="A61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -1869,7 +1881,7 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23">
       <c r="A62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -1890,7 +1902,7 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23">
       <c r="A63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -1911,7 +1923,7 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23">
       <c r="A64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -1932,7 +1944,7 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23">
       <c r="A65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -1953,7 +1965,7 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23">
       <c r="A66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -1974,7 +1986,7 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23">
       <c r="A67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -1995,7 +2007,7 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23">
       <c r="A68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2016,7 +2028,7 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23">
       <c r="A69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -2037,7 +2049,7 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23">
       <c r="A70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2058,7 +2070,7 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23">
       <c r="A71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2079,7 +2091,7 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23">
       <c r="A72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2100,7 +2112,7 @@
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23">
       <c r="A73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -2121,7 +2133,7 @@
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23">
       <c r="A74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -2142,7 +2154,7 @@
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23">
       <c r="A75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -2163,7 +2175,7 @@
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23">
       <c r="A76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -2184,7 +2196,7 @@
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23">
       <c r="A77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -2193,7 +2205,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23">
       <c r="A78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -2202,7 +2214,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23">
       <c r="A79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2218,19 +2230,20 @@
     <hyperlink ref="C6" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add ManagePageUserModel and ChangePasswordTests
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="DataSet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -83,10 +84,58 @@
     <t>b676KK</t>
   </si>
   <si>
-    <t>LogInValidEmail</t>
+    <t>a</t>
   </si>
   <si>
-    <t>a</t>
+    <t>CurrentPassword</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ValidPasswordChange</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutCurrentPassword</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>ValidLogin</t>
+  </si>
+  <si>
+    <t>ValidLogin2</t>
+  </si>
+  <si>
+    <t>b@b.b</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithWrongCurrentPassword</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutNewPassword</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutConfirmPassword</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutData</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithInvalidSymbols</t>
+  </si>
+  <si>
+    <t>&lt;/</t>
   </si>
 </sst>
 </file>
@@ -147,12 +196,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -162,7 +226,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
@@ -170,6 +234,9 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -477,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -761,15 +828,8 @@
       <c r="W8" s="1"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="C9" s="6"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -2230,14 +2290,1656 @@
     <hyperlink ref="C6" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="A25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="A26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="A27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="A28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="A29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="A30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="A31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="A32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="1:24">
+      <c r="A33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="A34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="1:24">
+      <c r="A35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="1:24">
+      <c r="A36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="1:24">
+      <c r="A37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="1:24">
+      <c r="A38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="1:24">
+      <c r="A39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="1:24">
+      <c r="A40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="1:24">
+      <c r="A41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="1:24">
+      <c r="A42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+    </row>
+    <row r="43" spans="1:24">
+      <c r="A43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="1:24">
+      <c r="A44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="1:24">
+      <c r="A45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+    </row>
+    <row r="46" spans="1:24">
+      <c r="A46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+    </row>
+    <row r="47" spans="1:24">
+      <c r="A47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="1:24">
+      <c r="A48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="1:24">
+      <c r="A49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="A50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="1:24">
+      <c r="A51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="1:24">
+      <c r="A52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+    </row>
+    <row r="53" spans="1:24">
+      <c r="A53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+    </row>
+    <row r="54" spans="1:24">
+      <c r="A54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+    </row>
+    <row r="55" spans="1:24">
+      <c r="A55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+    </row>
+    <row r="56" spans="1:24">
+      <c r="A56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+    </row>
+    <row r="57" spans="1:24">
+      <c r="A57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+    </row>
+    <row r="58" spans="1:24">
+      <c r="A58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+    </row>
+    <row r="59" spans="1:24">
+      <c r="A59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+    </row>
+    <row r="60" spans="1:24">
+      <c r="A60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+    </row>
+    <row r="61" spans="1:24">
+      <c r="A61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+    </row>
+    <row r="62" spans="1:24">
+      <c r="A62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+    </row>
+    <row r="63" spans="1:24">
+      <c r="A63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+    </row>
+    <row r="64" spans="1:24">
+      <c r="A64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+    </row>
+    <row r="65" spans="1:24">
+      <c r="A65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+    </row>
+    <row r="66" spans="1:24">
+      <c r="A66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+    </row>
+    <row r="67" spans="1:24">
+      <c r="A67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+    </row>
+    <row r="68" spans="1:24">
+      <c r="A68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+    </row>
+    <row r="69" spans="1:24">
+      <c r="A69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+    </row>
+    <row r="70" spans="1:24">
+      <c r="A70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+    </row>
+    <row r="71" spans="1:24">
+      <c r="A71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+    </row>
+    <row r="72" spans="1:24">
+      <c r="A72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+    </row>
+    <row r="73" spans="1:24">
+      <c r="A73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
ManagePage changes valid login password change
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
@@ -186,7 +186,7 @@
     <t>UserEmail</t>
   </si>
   <si>
-    <t>ValidLoginReset</t>
+    <t>ValidPasswordChangeReset</t>
   </si>
 </sst>
 </file>
@@ -2367,7 +2367,7 @@
   <dimension ref="A1:AB74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
AdminPage = some tests/5 fail for srs/
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/RegisterPageData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -174,9 +174,6 @@
     <t>afdbf879-0704-4fd5-a2d2-0528f109eebe</t>
   </si>
   <si>
-    <t>EditUser</t>
-  </si>
-  <si>
     <t>RoleAdmin</t>
   </si>
   <si>
@@ -187,6 +184,42 @@
   </si>
   <si>
     <t>ValidPasswordChangeReset</t>
+  </si>
+  <si>
+    <t>ManagePage</t>
+  </si>
+  <si>
+    <t>AdminPage</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdmin</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdminWithoutPassword</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdminWithoutConfirmPassword</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdminWithoutFullName</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdminWithoutAnyData</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdminWithTwoRoles</t>
+  </si>
+  <si>
+    <t>EditUserInfoByAdminWithoutPasswordMatch</t>
+  </si>
+  <si>
+    <t>Delete user</t>
+  </si>
+  <si>
+    <t>Delete admin</t>
   </si>
 </sst>
 </file>
@@ -246,7 +279,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +289,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +335,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
@@ -298,11 +343,13 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -2364,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB74"/>
+  <dimension ref="A1:AB83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2384,37 +2431,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="12" t="s">
         <v>43</v>
       </c>
       <c r="L1" s="1"/>
@@ -2436,23 +2483,19 @@
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="A2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="12"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -2472,25 +2515,23 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="8"/>
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -2510,25 +2551,25 @@
       <c r="AB3" s="1"/>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11" t="s">
+      <c r="A4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="H4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -2548,23 +2589,25 @@
       <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="A5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -2584,23 +2627,23 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="8"/>
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -2620,25 +2663,23 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="A7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -2658,23 +2699,25 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -2694,23 +2737,23 @@
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2730,19 +2773,23 @@
       <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -2762,25 +2809,19 @@
       <c r="AB10" s="1"/>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="A11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2800,23 +2841,25 @@
       <c r="AB11" s="1"/>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="A12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2836,28 +2879,38 @@
       <c r="AB12" s="1"/>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="10" t="s">
-        <v>45</v>
+      <c r="J13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2878,23 +2931,19 @@
       <c r="AB13" s="1"/>
     </row>
     <row r="14" spans="1:28">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="A14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2914,23 +2963,23 @@
       <c r="AB14" s="1"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="A15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -2950,8 +2999,33 @@
       <c r="AB15" s="1"/>
     </row>
     <row r="16" spans="1:28">
-      <c r="A16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="A16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2971,8 +3045,25 @@
       <c r="AB16" s="1"/>
     </row>
     <row r="17" spans="1:28">
-      <c r="A17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="A17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="9"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -2992,8 +3083,25 @@
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28">
-      <c r="A18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="A18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -3013,8 +3121,27 @@
       <c r="AB18" s="1"/>
     </row>
     <row r="19" spans="1:28">
-      <c r="A19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="A19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -3034,8 +3161,23 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="A20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -3055,8 +3197,31 @@
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="A21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="9"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -3076,8 +3241,27 @@
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="A22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -3097,8 +3281,23 @@
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -3118,8 +3317,23 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -3139,8 +3353,19 @@
       <c r="AB24" s="1"/>
     </row>
     <row r="25" spans="1:28">
-      <c r="A25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="A25" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -3160,8 +3385,19 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28">
-      <c r="A26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="A26" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -4133,6 +4369,18 @@
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="1"/>
     </row>
     <row r="73" spans="1:28">
       <c r="A73" s="1"/>
@@ -4142,6 +4390,18 @@
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
     </row>
     <row r="74" spans="1:28">
       <c r="A74" s="1"/>
@@ -4151,19 +4411,196 @@
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+    </row>
+    <row r="75" spans="1:28">
+      <c r="A75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+    </row>
+    <row r="76" spans="1:28">
+      <c r="A76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
+    </row>
+    <row r="77" spans="1:28">
+      <c r="A77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+      <c r="AA77" s="1"/>
+      <c r="AB77" s="1"/>
+    </row>
+    <row r="78" spans="1:28">
+      <c r="A78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="Z78" s="1"/>
+      <c r="AA78" s="1"/>
+      <c r="AB78" s="1"/>
+    </row>
+    <row r="79" spans="1:28">
+      <c r="A79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+      <c r="Y79" s="1"/>
+      <c r="Z79" s="1"/>
+      <c r="AA79" s="1"/>
+      <c r="AB79" s="1"/>
+    </row>
+    <row r="80" spans="1:28">
+      <c r="A80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
+      <c r="Z80" s="1"/>
+      <c r="AA80" s="1"/>
+      <c r="AB80" s="1"/>
+    </row>
+    <row r="81" spans="1:16">
+      <c r="A81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+    </row>
+    <row r="82" spans="1:16">
+      <c r="A82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+    </row>
+    <row r="83" spans="1:16">
+      <c r="A83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B12" r:id="rId3"/>
-    <hyperlink ref="B13" r:id="rId4"/>
-    <hyperlink ref="B14" r:id="rId5"/>
-    <hyperlink ref="B15" r:id="rId6"/>
-    <hyperlink ref="C13" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B15" r:id="rId3"/>
+    <hyperlink ref="B16" r:id="rId4"/>
+    <hyperlink ref="B23" r:id="rId5"/>
+    <hyperlink ref="B24" r:id="rId6"/>
+    <hyperlink ref="C16" r:id="rId7"/>
+    <hyperlink ref="B17" r:id="rId8"/>
+    <hyperlink ref="C17" r:id="rId9"/>
+    <hyperlink ref="B18" r:id="rId10"/>
+    <hyperlink ref="C18" r:id="rId11"/>
+    <hyperlink ref="B19" r:id="rId12"/>
+    <hyperlink ref="C19" r:id="rId13"/>
+    <hyperlink ref="B20" r:id="rId14"/>
+    <hyperlink ref="C20" r:id="rId15"/>
+    <hyperlink ref="B21" r:id="rId16"/>
+    <hyperlink ref="B22" r:id="rId17"/>
+    <hyperlink ref="C21" r:id="rId18"/>
+    <hyperlink ref="C22" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>